<commit_message>
qut_experiments file modified to be consistent with the parameters file used in the soiling_model. some parameters are still missing, but are not used
</commit_message>
<xml_diff>
--- a/data/public/qut_experiments/parameters_qut_experiments.xlsx
+++ b/data/public/qut_experiments/parameters_qut_experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cholette\Dropbox\research\toolboxes_and_code\python_soiling_model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovanni\Dropbox\Python Soiling Models\HelioSoil\data\public\qut_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B667DA-41F4-406F-845E-3D8DD93B1DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A0435C-FC61-4177-A66D-EF829A2C4912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20640" yWindow="540" windowWidth="18420" windowHeight="11772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
   <si>
     <t>Parameter</t>
   </si>
@@ -272,6 +272,21 @@
   </si>
   <si>
     <t>minimum, maximum, number of bins (log spacing)</t>
+  </si>
+  <si>
+    <t>SITE</t>
+  </si>
+  <si>
+    <t>DUST</t>
+  </si>
+  <si>
+    <t>PLANT</t>
+  </si>
+  <si>
+    <t>HELIOSTATS</t>
+  </si>
+  <si>
+    <t>CONSTANTS</t>
   </si>
 </sst>
 </file>
@@ -281,7 +296,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +427,15 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -758,10 +782,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1117,263 +1143,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>-27.477436388009799</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>153.02737396909501</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>153.02737396909501</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
         <v>82</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>80</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B11">
+      <c r="B14">
         <v>2000</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B15" s="1">
         <v>8.5000000000000005E-20</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B13">
+      <c r="B16">
         <v>0.17</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B17" s="1">
         <v>72400000000</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>29</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16">
-        <v>114.9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="1">
-        <v>6.5000000000000003E-20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18">
-        <v>0.27</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="1">
-        <v>80100000000</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -1385,186 +1385,239 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21">
+        <v>114.9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1">
+        <v>6.5000000000000003E-20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24">
+        <v>0.27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1">
+        <v>80100000000</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="B21">
+      <c r="B27">
         <v>1.2047000000000001</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C27" t="s">
         <v>40</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="B22">
+      <c r="B28">
         <v>1.8170000000000001E-5</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C28" t="s">
         <v>43</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>45</v>
       </c>
-      <c r="B23">
+      <c r="B29">
         <v>6.5E-8</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C29" t="s">
         <v>34</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>47</v>
       </c>
-      <c r="B24">
+      <c r="B30">
         <v>1367.7</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C30" t="s">
         <v>48</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>50</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B31" t="s">
         <v>51</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B32" s="2">
         <v>1.3809999999999999E-23</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C32" t="s">
         <v>54</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>56</v>
       </c>
-      <c r="B27">
+      <c r="B33">
         <v>0.4</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D33" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28">
-        <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>60</v>
       </c>
-      <c r="B29">
+      <c r="B34">
         <v>1000</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>62</v>
       </c>
-      <c r="B30">
+      <c r="B35">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>64</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B36" t="s">
         <v>65</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D36" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>67</v>
       </c>
-      <c r="B32">
+      <c r="B37">
         <v>400</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D37" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>69</v>
       </c>
-      <c r="B33">
+      <c r="B38">
         <v>2</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D38" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
         <v>70</v>
       </c>
-      <c r="B34">
+      <c r="B39">
         <v>3</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D39" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B40" s="1">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C40" t="s">
         <v>34</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D40" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
little edits to fix typos and adding a line in the notebook to show area deposition flux
</commit_message>
<xml_diff>
--- a/data/public/qut_experiments/parameters_qut_experiments.xlsx
+++ b/data/public/qut_experiments/parameters_qut_experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovanni\Dropbox\Python Soiling Models\HelioSoil\data\public\qut_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A0435C-FC61-4177-A66D-EF829A2C4912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A463924-0260-4578-B95A-A0539E27D8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20640" yWindow="540" windowWidth="18420" windowHeight="11772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15563" yWindow="3180" windowWidth="21599" windowHeight="11423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>location_name</t>
   </si>
   <si>
-    <t>Woomera</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>CONSTANTS</t>
+  </si>
+  <si>
+    <t>Brisbane</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1146,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -1181,444 +1181,444 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>-27.477436388009799</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>153.02737396909501</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7">
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
         <v>80</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>2000</v>
       </c>
       <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
         <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1">
         <v>8.5000000000000005E-20</v>
       </c>
       <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
         <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <v>0.17</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1">
         <v>72400000000</v>
       </c>
       <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
         <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
         <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <v>114.9</v>
       </c>
       <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
         <v>34</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1">
         <v>6.5000000000000003E-20</v>
       </c>
       <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
         <v>24</v>
-      </c>
-      <c r="D23" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>0.27</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1">
         <v>80100000000</v>
       </c>
       <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
         <v>29</v>
-      </c>
-      <c r="D25" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27">
         <v>1.2047000000000001</v>
       </c>
       <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
         <v>40</v>
-      </c>
-      <c r="D27" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28">
         <v>1.8170000000000001E-5</v>
       </c>
       <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
         <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>6.5E-8</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30">
         <v>1367.7</v>
       </c>
       <c r="C30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" t="s">
         <v>48</v>
-      </c>
-      <c r="D30" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
         <v>50</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>51</v>
-      </c>
-      <c r="D31" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" s="2">
         <v>1.3809999999999999E-23</v>
       </c>
       <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" t="s">
         <v>54</v>
-      </c>
-      <c r="D32" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33">
         <v>0.4</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34">
         <v>1000</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
         <v>64</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>65</v>
-      </c>
-      <c r="D36" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37">
         <v>400</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B40" s="1">
         <v>4.0000000000000001E-10</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>